<commit_message>
scrollbar fixed while navigating
</commit_message>
<xml_diff>
--- a/utils/pin_submit/pin_temp/train.xlsx
+++ b/utils/pin_submit/pin_temp/train.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SRR\Riga Express\_Docs\04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SRR\Riga Express\_Docs\06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE726CC-5DA4-44CE-A24E-29A81D512E0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E4325BC-40D9-4FA4-AB91-3C6055D1723D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E378575C-15C9-4283-B2D7-7706E0C2694D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0AD296B7-7041-44C7-9356-2F666910BFFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,21 +31,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>CMAU6137459</t>
-  </si>
-  <si>
-    <t>;DOLVA00063681</t>
-  </si>
-  <si>
-    <t>APZU4309717</t>
-  </si>
-  <si>
-    <t>;DOLVA00063682</t>
-  </si>
-  <si>
-    <t>APZU4614080</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+  <si>
+    <t>CMAU9099877</t>
+  </si>
+  <si>
+    <t>;DOLVA00063742</t>
+  </si>
+  <si>
+    <t>CAIU8312898</t>
+  </si>
+  <si>
+    <t>TEMU6437272</t>
+  </si>
+  <si>
+    <t>FCIU9169820</t>
+  </si>
+  <si>
+    <t>BMOU6720890</t>
+  </si>
+  <si>
+    <t>TRLU4885536</t>
+  </si>
+  <si>
+    <t>CMAU7128390</t>
+  </si>
+  <si>
+    <t>TGHU6321448</t>
+  </si>
+  <si>
+    <t>TGHU9515160</t>
+  </si>
+  <si>
+    <t>TCNU3409791</t>
+  </si>
+  <si>
+    <t>TCLU6716222</t>
+  </si>
+  <si>
+    <t>GESU4748994</t>
+  </si>
+  <si>
+    <t>;DOLVA00063818</t>
+  </si>
+  <si>
+    <t>CMAU7813497</t>
+  </si>
+  <si>
+    <t>;DOLVA00063855</t>
+  </si>
+  <si>
+    <t>TLLU4566625</t>
+  </si>
+  <si>
+    <t>;DOLVA00063817</t>
+  </si>
+  <si>
+    <t>APZU4718696</t>
+  </si>
+  <si>
+    <t>;DOLVA00063878</t>
+  </si>
+  <si>
+    <t>CAIU7117840</t>
+  </si>
+  <si>
+    <t>;DOLVA00063820</t>
+  </si>
+  <si>
+    <t>CMAU9010489</t>
+  </si>
+  <si>
+    <t>;DOLVA00063879</t>
+  </si>
+  <si>
+    <t>ECMU9757564</t>
+  </si>
+  <si>
+    <t>;DOLVA00063782</t>
+  </si>
+  <si>
+    <t>TGBU5575981</t>
+  </si>
+  <si>
+    <t>;DOLVA00063852</t>
+  </si>
+  <si>
+    <t>MRKU4918940</t>
+  </si>
+  <si>
+    <t>;704851</t>
+  </si>
+  <si>
+    <t>MRKU6111026</t>
+  </si>
+  <si>
+    <t>;869034</t>
+  </si>
+  <si>
+    <t>APHU6741856</t>
+  </si>
+  <si>
+    <t>;DOLVA00063900</t>
   </si>
 </sst>
 </file>
@@ -417,11 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C72B3E6-3630-41D5-9783-C54FDD053201}">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AE5F74-7635-49D6-AF3D-F2F65E30B4C3}">
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,79 +526,171 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A18">
+  <conditionalFormatting sqref="A1:A22">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>